<commit_message>
fix bug add locals
</commit_message>
<xml_diff>
--- a/resources/wording.xlsx
+++ b/resources/wording.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="44">
   <si>
     <t>Translation Table</t>
   </si>
@@ -99,6 +99,51 @@
   </si>
   <si>
     <t>＜　Cancel</t>
+  </si>
+  <si>
+    <t>戻る</t>
+  </si>
+  <si>
+    <t>error_header</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>connection_error</t>
+  </si>
+  <si>
+    <t>Connection error</t>
+  </si>
+  <si>
+    <t>failed_header</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>incorrect_password_error</t>
+  </si>
+  <si>
+    <t>Incorrect password</t>
+  </si>
+  <si>
+    <t>recover_password_alert_header</t>
+  </si>
+  <si>
+    <t>Nice</t>
+  </si>
+  <si>
+    <t>recover_password_alert_msg</t>
+  </si>
+  <si>
+    <t>Sent</t>
+  </si>
+  <si>
+    <t>alert_button_ok</t>
+  </si>
+  <si>
+    <t>OK</t>
   </si>
 </sst>
 </file>
@@ -390,7 +435,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -445,10 +490,13 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1727,108 +1775,136 @@
         <v>28</v>
       </c>
       <c r="C12" t="s" s="14">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="9"/>
     </row>
     <row r="13" ht="20.35" customHeight="1">
-      <c r="A13" s="18"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="19"/>
+      <c r="A13" t="s" s="13">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s" s="14">
+        <v>31</v>
+      </c>
+      <c r="C13" s="18"/>
       <c r="D13" s="8"/>
       <c r="E13" s="9"/>
     </row>
     <row r="14" ht="20.35" customHeight="1">
-      <c r="A14" s="18"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="19"/>
+      <c r="A14" t="s" s="13">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s" s="14">
+        <v>33</v>
+      </c>
+      <c r="C14" s="18"/>
       <c r="D14" s="8"/>
       <c r="E14" s="9"/>
     </row>
     <row r="15" ht="20.35" customHeight="1">
-      <c r="A15" s="18"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="19"/>
+      <c r="A15" t="s" s="19">
+        <v>34</v>
+      </c>
+      <c r="B15" t="s" s="15">
+        <v>35</v>
+      </c>
+      <c r="C15" s="18"/>
       <c r="D15" s="8"/>
       <c r="E15" s="9"/>
     </row>
     <row r="16" ht="20.35" customHeight="1">
-      <c r="A16" s="18"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="19"/>
+      <c r="A16" t="s" s="19">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s" s="15">
+        <v>37</v>
+      </c>
+      <c r="C16" s="18"/>
       <c r="D16" s="8"/>
       <c r="E16" s="9"/>
     </row>
-    <row r="17" ht="20.35" customHeight="1">
-      <c r="A17" s="18"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="19"/>
+    <row r="17" ht="27" customHeight="1">
+      <c r="A17" t="s" s="13">
+        <v>38</v>
+      </c>
+      <c r="B17" t="s" s="14">
+        <v>39</v>
+      </c>
+      <c r="C17" s="18"/>
       <c r="D17" s="8"/>
       <c r="E17" s="9"/>
     </row>
-    <row r="18" ht="20.35" customHeight="1">
-      <c r="A18" s="18"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="19"/>
+    <row r="18" ht="27" customHeight="1">
+      <c r="A18" t="s" s="13">
+        <v>40</v>
+      </c>
+      <c r="B18" t="s" s="14">
+        <v>41</v>
+      </c>
+      <c r="C18" s="18"/>
       <c r="D18" s="8"/>
       <c r="E18" s="9"/>
     </row>
     <row r="19" ht="20.35" customHeight="1">
-      <c r="A19" s="18"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="19"/>
+      <c r="A19" t="s" s="13">
+        <v>42</v>
+      </c>
+      <c r="B19" t="s" s="14">
+        <v>43</v>
+      </c>
+      <c r="C19" s="18"/>
       <c r="D19" s="8"/>
       <c r="E19" s="9"/>
     </row>
     <row r="20" ht="20.35" customHeight="1">
-      <c r="A20" s="18"/>
+      <c r="A20" s="20"/>
       <c r="B20" s="16"/>
-      <c r="C20" s="19"/>
+      <c r="C20" s="18"/>
       <c r="D20" s="8"/>
       <c r="E20" s="9"/>
     </row>
     <row r="21" ht="20.35" customHeight="1">
-      <c r="A21" s="18"/>
+      <c r="A21" s="20"/>
       <c r="B21" s="16"/>
-      <c r="C21" s="19"/>
+      <c r="C21" s="18"/>
       <c r="D21" s="8"/>
       <c r="E21" s="9"/>
     </row>
     <row r="22" ht="20.35" customHeight="1">
-      <c r="A22" s="18"/>
+      <c r="A22" s="20"/>
       <c r="B22" s="16"/>
-      <c r="C22" s="19"/>
+      <c r="C22" s="18"/>
       <c r="D22" s="8"/>
       <c r="E22" s="9"/>
     </row>
     <row r="23" ht="20.35" customHeight="1">
-      <c r="A23" s="18"/>
+      <c r="A23" s="20"/>
       <c r="B23" s="16"/>
-      <c r="C23" s="19"/>
+      <c r="C23" s="18"/>
       <c r="D23" s="8"/>
       <c r="E23" s="9"/>
     </row>
     <row r="24" ht="20.35" customHeight="1">
-      <c r="A24" s="18"/>
+      <c r="A24" s="20"/>
       <c r="B24" s="16"/>
-      <c r="C24" s="19"/>
+      <c r="C24" s="18"/>
       <c r="D24" s="8"/>
       <c r="E24" s="9"/>
     </row>
     <row r="25" ht="20.35" customHeight="1">
-      <c r="A25" s="18"/>
+      <c r="A25" s="20"/>
       <c r="B25" s="16"/>
-      <c r="C25" s="19"/>
+      <c r="C25" s="18"/>
       <c r="D25" s="8"/>
       <c r="E25" s="9"/>
     </row>
     <row r="26" ht="20.35" customHeight="1">
-      <c r="A26" s="18"/>
+      <c r="A26" s="20"/>
       <c r="B26" s="16"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="21"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Update wording and fix crash bug in recover screen
</commit_message>
<xml_diff>
--- a/resources/wording.xlsx
+++ b/resources/wording.xlsx
@@ -29,7 +29,7 @@
     <t>login</t>
   </si>
   <si>
-    <t>Login  ＞</t>
+    <t>Login</t>
   </si>
   <si>
     <t>ログイン</t>
@@ -95,7 +95,7 @@
     <t>cancel</t>
   </si>
   <si>
-    <t>＜　Cancel</t>
+    <t>Cancel</t>
   </si>
   <si>
     <t>戻る</t>

</xml_diff>

<commit_message>
update wording to add ja recover_password text
</commit_message>
<xml_diff>
--- a/resources/wording.xlsx
+++ b/resources/wording.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="50">
   <si>
     <t>Translation Table</t>
   </si>
@@ -29,7 +29,7 @@
     <t>login</t>
   </si>
   <si>
-    <t>Login</t>
+    <t>Login  ＞</t>
   </si>
   <si>
     <t>ログイン</t>
@@ -92,10 +92,13 @@
     <t>Recover Password</t>
   </si>
   <si>
+    <t>送信</t>
+  </si>
+  <si>
     <t>cancel</t>
   </si>
   <si>
-    <t>Cancel</t>
+    <t>＜　Cancel</t>
   </si>
   <si>
     <t>戻る</t>
@@ -138,6 +141,9 @@
   </si>
   <si>
     <t>recover_password_alert_header</t>
+  </si>
+  <si>
+    <t>Nice</t>
   </si>
   <si>
     <t>完了</t>
@@ -1784,108 +1790,112 @@
       <c r="B11" t="s" s="14">
         <v>25</v>
       </c>
-      <c r="C11" s="17"/>
+      <c r="C11" t="s" s="17">
+        <v>26</v>
+      </c>
       <c r="D11" s="8"/>
       <c r="E11" s="9"/>
     </row>
     <row r="12" ht="20.25" customHeight="1">
       <c r="A12" t="s" s="13">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s" s="18">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s" s="19">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="9"/>
     </row>
     <row r="13" ht="20.25" customHeight="1">
       <c r="A13" t="s" s="13">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s" s="14">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C13" t="s" s="15">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="9"/>
     </row>
     <row r="14" ht="20.25" customHeight="1">
       <c r="A14" t="s" s="13">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s" s="14">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s" s="15">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="9"/>
     </row>
     <row r="15" ht="20.25" customHeight="1">
       <c r="A15" t="s" s="20">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s" s="17">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C15" t="s" s="15">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="9"/>
     </row>
     <row r="16" ht="20.25" customHeight="1">
       <c r="A16" t="s" s="20">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B16" t="s" s="17">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C16" t="s" s="15">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="9"/>
     </row>
     <row r="17" ht="27" customHeight="1">
       <c r="A17" t="s" s="13">
-        <v>41</v>
-      </c>
-      <c r="B17" s="14"/>
+        <v>42</v>
+      </c>
+      <c r="B17" t="s" s="14">
+        <v>43</v>
+      </c>
       <c r="C17" t="s" s="15">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="9"/>
     </row>
     <row r="18" ht="27" customHeight="1">
       <c r="A18" t="s" s="13">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B18" t="s" s="14">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s" s="15">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="9"/>
     </row>
     <row r="19" ht="20.25" customHeight="1">
       <c r="A19" t="s" s="13">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B19" t="s" s="14">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C19" t="s" s="15">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="9"/>

</xml_diff>